<commit_message>
Features: Corrección en la generación de la...
lista de citas por periodo, en formato excel
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/appointment.xlsx
+++ b/src/main/resources/templates/appointment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\scimec\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4E8433-A062-4EDB-91D3-C24B443BBAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C237A0DB-F098-40AE-8840-C44140854A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9045213E-3626-4F8C-BE92-1E6318E25160}"/>
   </bookViews>
@@ -169,11 +169,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -495,7 +495,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,21 +509,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="10"/>
-      <c r="C2" s="7"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -906,8 +906,9 @@
       <c r="F46" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>